<commit_message>
Implement failure cases for RRI. Closes #60
</commit_message>
<xml_diff>
--- a/tests/ExcelFinancialFunctions.Tests/testdata/testdata.xlsx
+++ b/tests/ExcelFinancialFunctions.Tests/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\fsprojects\ExcelFinancialFunctions\tests\ExcelFinancialFunctions.Tests\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906479D4-E9D6-40E7-96FF-687FEB3E60EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5FF58E27-E268-4CF6-B76B-8B2D72ED41D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12400" yWindow="5370" windowWidth="21610" windowHeight="14360" xr2:uid="{EC39768B-AFC7-444D-B9A8-53DEC24456B9}"/>
   </bookViews>
@@ -101,8 +101,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DF0E49A7-8B55-4120-AE6D-65AEA00C5802}" name="Table1" displayName="Table1" ref="A1:D25" totalsRowShown="0">
-  <autoFilter ref="A1:D25" xr:uid="{DF0E49A7-8B55-4120-AE6D-65AEA00C5802}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DF0E49A7-8B55-4120-AE6D-65AEA00C5802}" name="Table1" displayName="Table1" ref="A1:D32" totalsRowShown="0">
+  <autoFilter ref="A1:D32" xr:uid="{DF0E49A7-8B55-4120-AE6D-65AEA00C5802}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{2F7BD33E-C616-464E-9B4D-5B9D4629B575}" name="nper"/>
     <tableColumn id="2" xr3:uid="{97C02E16-CE21-4F1C-9A8F-7E0DF4AD8BC8}" name="pv"/>
@@ -412,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C28EAF-B24A-4C1D-9842-A03F9323BA2D}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -439,28 +439,28 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D25" si="0">_xlfn.RRI(A2,B2,C2)</f>
-        <v>0</v>
+        <v>400</v>
+      </c>
+      <c r="D2" t="e">
+        <f>_xlfn.RRI(A2,B2,C2)</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C3">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="D3" t="e">
         <f>_xlfn.RRI(A3,B3,C3)</f>
@@ -469,330 +469,435 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>-1</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>-3</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>_xlfn.RRI(A4,B4,C4)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>_xlfn.RRI(A5,B5,C5)</f>
+        <v>-0.17459581473198149</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>-0.5</v>
+        <v>-90</v>
+      </c>
+      <c r="D6" t="e">
+        <f>_xlfn.RRI(A6,B6,C6)</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>-1</v>
+        <f t="shared" ref="D7:D32" si="0">_xlfn.RRI(A7,B7,C7)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D8" t="e">
-        <f t="shared" si="0"/>
+        <f>_xlfn.RRI(A8,B8,C8)</f>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B9">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>-1</v>
+        <v>10</v>
       </c>
       <c r="D9">
-        <f>_xlfn.RRI(A9,B9,C9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <v>300</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>300</v>
+        <v>8</v>
       </c>
       <c r="D10">
-        <f>_xlfn.RRI(A10,B10,C10)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B11">
-        <v>300</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>400</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>2.426318074098921E-2</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B12">
-        <v>300</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>0.24092317318260137</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B13">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>40000</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>0.50341274654387536</v>
+        <v>10</v>
+      </c>
+      <c r="D13" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>300</v>
+        <v>-5</v>
       </c>
       <c r="C14">
-        <v>400</v>
+        <v>-6</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>1.2058882052318642E-2</v>
+        <f>_xlfn.RRI(A14,B14,C14)</f>
+        <v>1.5309470499731193E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="B15">
-        <v>300</v>
+        <v>-5</v>
       </c>
       <c r="C15">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>0.11396731243901459</v>
+        <f>_xlfn.RRI(A15,B15,C15)</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B16">
-        <v>300</v>
+        <v>-1</v>
       </c>
       <c r="C16">
-        <v>40000</v>
+        <v>-1</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>0.22613732776711237</v>
+        <f>_xlfn.RRI(A16,B16,C16)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B17">
         <v>300</v>
       </c>
       <c r="C17">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>7.5993101546305564E-3</v>
+        <f>_xlfn.RRI(A17,B17,C17)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B18">
         <v>300</v>
       </c>
       <c r="C18">
-        <v>4000</v>
+        <v>400</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>7.0541853470322824E-2</v>
+        <v>2.426318074098921E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B19">
         <v>300</v>
       </c>
       <c r="C19">
-        <v>40000</v>
+        <v>4000</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>0.13741628093790048</v>
+        <v>0.24092317318260137</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B20">
-        <v>10000</v>
+        <v>300</v>
       </c>
       <c r="C20">
-        <v>2441880</v>
+        <v>40000</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>0.98822504304098735</v>
+        <v>0.50341274654387536</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B21">
-        <v>5000</v>
+        <v>300</v>
       </c>
       <c r="C21">
-        <v>6000</v>
+        <v>400</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>4.6635139392105618E-2</v>
+        <v>1.2058882052318642E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B22">
-        <v>5000</v>
+        <v>300</v>
       </c>
       <c r="C22">
-        <v>10000</v>
+        <v>4000</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>0.18920711500272103</v>
+        <v>0.11396731243901459</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B23">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="C23">
-        <v>275</v>
+        <v>40000</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>0.10000000000000009</v>
+        <v>0.22613732776711237</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="B24">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="C24">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>0.41421356237309492</v>
+        <v>7.5993101546305564E-3</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
+        <v>38</v>
+      </c>
+      <c r="B25">
+        <v>300</v>
+      </c>
+      <c r="C25">
+        <v>4000</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>7.0541853470322824E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>38</v>
+      </c>
+      <c r="B26">
+        <v>300</v>
+      </c>
+      <c r="C26">
+        <v>40000</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>0.13741628093790048</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>10000</v>
+      </c>
+      <c r="C27">
+        <v>2441880</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>0.98822504304098735</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>5000</v>
+      </c>
+      <c r="C28">
+        <v>6000</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>4.6635139392105618E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>5000</v>
+      </c>
+      <c r="C29">
+        <v>10000</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>0.18920711500272103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>250</v>
+      </c>
+      <c r="C30">
+        <v>275</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>0.10000000000000009</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>250</v>
+      </c>
+      <c r="C31">
+        <v>500</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>0.41421356237309492</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32">
         <v>3</v>
       </c>
-      <c r="B25">
+      <c r="B32">
         <v>250</v>
       </c>
-      <c r="C25">
+      <c r="C32">
         <v>880</v>
       </c>
-      <c r="D25">
+      <c r="D32">
         <f t="shared" si="0"/>
         <v>0.5211809843045565</v>
       </c>

</xml_diff>

<commit_message>
Add test data for pduration. Begins #62
</commit_message>
<xml_diff>
--- a/tests/ExcelFinancialFunctions.Tests/testdata/testdata.xlsx
+++ b/tests/ExcelFinancialFunctions.Tests/testdata/testdata.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\fsprojects\ExcelFinancialFunctions\tests\ExcelFinancialFunctions.Tests\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5FF58E27-E268-4CF6-B76B-8B2D72ED41D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41E4799-5481-4477-87B4-42B6D97F4765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12400" yWindow="5370" windowWidth="21610" windowHeight="14360" xr2:uid="{EC39768B-AFC7-444D-B9A8-53DEC24456B9}"/>
+    <workbookView xWindow="8540" yWindow="3960" windowWidth="21610" windowHeight="14360" activeTab="1" xr2:uid="{EC39768B-AFC7-444D-B9A8-53DEC24456B9}"/>
   </bookViews>
   <sheets>
     <sheet name="rri" sheetId="1" r:id="rId1"/>
+    <sheet name="pduration" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>nper</t>
   </si>
@@ -46,6 +47,12 @@
   </si>
   <si>
     <t>rri</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>pduration</t>
   </si>
 </sst>
 </file>
@@ -109,6 +116,21 @@
     <tableColumn id="3" xr3:uid="{DE9FD564-D130-44BA-8664-D2606A16C065}" name="fv"/>
     <tableColumn id="4" xr3:uid="{C5522036-5D17-4DE1-BB9B-8C5C0B6749C3}" name="rri">
       <calculatedColumnFormula>_xlfn.RRI(A2,B2,C2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BFC1A413-E1C7-425B-934D-F498CAA034AF}" name="Table2" displayName="Table2" ref="A1:D24" totalsRowShown="0">
+  <autoFilter ref="A1:D24" xr:uid="{BFC1A413-E1C7-425B-934D-F498CAA034AF}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{561856E1-824E-43BD-B4D4-6577D38CDCE6}" name="rate"/>
+    <tableColumn id="2" xr3:uid="{D0FB9E8E-C235-43EC-A4DE-95F419E81AF8}" name="pv"/>
+    <tableColumn id="3" xr3:uid="{C050AD2F-E77C-41A0-8FB1-F30463D3A078}" name="fv"/>
+    <tableColumn id="4" xr3:uid="{D1ECC235-BBEA-4C2D-B712-A4D7E5474809}" name="pduration">
+      <calculatedColumnFormula>_xlfn.PDURATION(A2,B2,C2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -414,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C28EAF-B24A-4C1D-9842-A03F9323BA2D}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D32" sqref="B14:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -908,4 +930,385 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A295A1-A566-4DB7-AE4A-33ED98E78A1E}">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="11.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1.5309470499731193E-2</v>
+      </c>
+      <c r="B2">
+        <v>-5</v>
+      </c>
+      <c r="C2">
+        <v>-6</v>
+      </c>
+      <c r="D2" t="e">
+        <f>_xlfn.PDURATION(A2,B2,C2)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>-1</v>
+      </c>
+      <c r="B3">
+        <v>-5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="e">
+        <f t="shared" ref="D3:D24" si="0">_xlfn.PDURATION(A3,B3,C3)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <v>-1</v>
+      </c>
+      <c r="D4" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>300</v>
+      </c>
+      <c r="C5">
+        <v>300</v>
+      </c>
+      <c r="D5" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>0.1</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>0.1</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2.426318074098921E-2</v>
+      </c>
+      <c r="B8">
+        <v>300</v>
+      </c>
+      <c r="C8">
+        <v>400</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>11.999999999999959</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>0.24092317318260137</v>
+      </c>
+      <c r="B9">
+        <v>300</v>
+      </c>
+      <c r="C9">
+        <v>4000</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>11.999999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>0.50341274654387536</v>
+      </c>
+      <c r="B10">
+        <v>300</v>
+      </c>
+      <c r="C10">
+        <v>40000</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>11.999999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>1.2058882052318642E-2</v>
+      </c>
+      <c r="B11">
+        <v>300</v>
+      </c>
+      <c r="C11">
+        <v>400</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>24.000000000000107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>0.11396731243901459</v>
+      </c>
+      <c r="B12">
+        <v>300</v>
+      </c>
+      <c r="C12">
+        <v>4000</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>24.000000000000014</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>0.22613732776711237</v>
+      </c>
+      <c r="B13">
+        <v>300</v>
+      </c>
+      <c r="C13">
+        <v>40000</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>24.000000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>7.5993101546305564E-3</v>
+      </c>
+      <c r="B14">
+        <v>300</v>
+      </c>
+      <c r="C14">
+        <v>400</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>38.000000000000433</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>7.0541853470322824E-2</v>
+      </c>
+      <c r="B15">
+        <v>300</v>
+      </c>
+      <c r="C15">
+        <v>4000</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>37.999999999999964</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>0.13741628093790048</v>
+      </c>
+      <c r="B16">
+        <v>300</v>
+      </c>
+      <c r="C16">
+        <v>40000</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>37.999999999999972</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>0.98822504304098735</v>
+      </c>
+      <c r="B17">
+        <v>10000</v>
+      </c>
+      <c r="C17">
+        <v>2441880</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>4.6635139392105618E-2</v>
+      </c>
+      <c r="B18">
+        <v>5000</v>
+      </c>
+      <c r="C18">
+        <v>6000</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>3.9999999999999618</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>0.18920711500272103</v>
+      </c>
+      <c r="B19">
+        <v>5000</v>
+      </c>
+      <c r="C19">
+        <v>10000</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000009</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="B20">
+        <v>250</v>
+      </c>
+      <c r="C20">
+        <v>275</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000075</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>0.41421356237309492</v>
+      </c>
+      <c r="B21">
+        <v>250</v>
+      </c>
+      <c r="C21">
+        <v>500</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>2.0000000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>0.5211809843045565</v>
+      </c>
+      <c r="B22">
+        <v>250</v>
+      </c>
+      <c r="C22">
+        <v>880</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>3.0000000000000009</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B23">
+        <v>2000</v>
+      </c>
+      <c r="C23">
+        <v>2200</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>3.8598661626226551</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <f>0.025/12</f>
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="B24">
+        <v>1000</v>
+      </c>
+      <c r="C24">
+        <v>1200</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>87.605476419371399</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement PDURATION. Finishes #62
</commit_message>
<xml_diff>
--- a/tests/ExcelFinancialFunctions.Tests/testdata/testdata.xlsx
+++ b/tests/ExcelFinancialFunctions.Tests/testdata/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\fsprojects\ExcelFinancialFunctions\tests\ExcelFinancialFunctions.Tests\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41E4799-5481-4477-87B4-42B6D97F4765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E5E1BF-E9B9-4ABA-947D-51D7FB3165EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8540" yWindow="3960" windowWidth="21610" windowHeight="14360" activeTab="1" xr2:uid="{EC39768B-AFC7-444D-B9A8-53DEC24456B9}"/>
+    <workbookView xWindow="3850" yWindow="2760" windowWidth="21610" windowHeight="14360" activeTab="1" xr2:uid="{EC39768B-AFC7-444D-B9A8-53DEC24456B9}"/>
   </bookViews>
   <sheets>
     <sheet name="rri" sheetId="1" r:id="rId1"/>
@@ -59,6 +59,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="169" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="172" formatCode="0.00000000000000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,13 +92,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="172" formatCode="0.00000000000000000"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -126,7 +136,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BFC1A413-E1C7-425B-934D-F498CAA034AF}" name="Table2" displayName="Table2" ref="A1:D24" totalsRowShown="0">
   <autoFilter ref="A1:D24" xr:uid="{BFC1A413-E1C7-425B-934D-F498CAA034AF}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{561856E1-824E-43BD-B4D4-6577D38CDCE6}" name="rate"/>
+    <tableColumn id="1" xr3:uid="{561856E1-824E-43BD-B4D4-6577D38CDCE6}" name="rate" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{D0FB9E8E-C235-43EC-A4DE-95F419E81AF8}" name="pv"/>
     <tableColumn id="3" xr3:uid="{C050AD2F-E77C-41A0-8FB1-F30463D3A078}" name="fv"/>
     <tableColumn id="4" xr3:uid="{D1ECC235-BBEA-4C2D-B712-A4D7E5474809}" name="pduration">
@@ -937,12 +947,13 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="11.08984375" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="4" max="4" width="20.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -960,7 +971,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1.5309470499731193E-2</v>
       </c>
       <c r="B2">
@@ -975,7 +986,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>-1</v>
       </c>
       <c r="B3">
@@ -990,7 +1001,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>0</v>
       </c>
       <c r="B4">
@@ -1005,7 +1016,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>0</v>
       </c>
       <c r="B5">
@@ -1020,7 +1031,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>0.1</v>
       </c>
       <c r="B6">
@@ -1035,7 +1046,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>0.1</v>
       </c>
       <c r="B7">
@@ -1050,7 +1061,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>2.426318074098921E-2</v>
       </c>
       <c r="B8">
@@ -1065,7 +1076,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>0.24092317318260137</v>
       </c>
       <c r="B9">
@@ -1080,7 +1091,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>0.50341274654387536</v>
       </c>
       <c r="B10">
@@ -1095,7 +1106,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>1.2058882052318642E-2</v>
       </c>
       <c r="B11">
@@ -1110,7 +1121,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>0.11396731243901459</v>
       </c>
       <c r="B12">
@@ -1125,7 +1136,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>0.22613732776711237</v>
       </c>
       <c r="B13">
@@ -1140,7 +1151,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>7.5993101546305564E-3</v>
       </c>
       <c r="B14">
@@ -1155,7 +1166,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="A15" s="2">
         <v>7.0541853470322824E-2</v>
       </c>
       <c r="B15">
@@ -1170,7 +1181,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16">
+      <c r="A16" s="2">
         <v>0.13741628093790048</v>
       </c>
       <c r="B16">
@@ -1185,7 +1196,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17">
+      <c r="A17" s="2">
         <v>0.98822504304098735</v>
       </c>
       <c r="B17">
@@ -1200,7 +1211,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18">
+      <c r="A18" s="2">
         <v>4.6635139392105618E-2</v>
       </c>
       <c r="B18">
@@ -1215,7 +1226,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="A19" s="2">
         <v>0.18920711500272103</v>
       </c>
       <c r="B19">
@@ -1230,7 +1241,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20">
+      <c r="A20" s="2">
         <v>0.10000000000000009</v>
       </c>
       <c r="B20">
@@ -1245,7 +1256,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21">
+      <c r="A21" s="2">
         <v>0.41421356237309492</v>
       </c>
       <c r="B21">
@@ -1260,7 +1271,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22">
+      <c r="A22" s="2">
         <v>0.5211809843045565</v>
       </c>
       <c r="B22">
@@ -1275,7 +1286,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23">
+      <c r="A23" s="2">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="B23">
@@ -1284,13 +1295,13 @@
       <c r="C23">
         <v>2200</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <f t="shared" si="0"/>
         <v>3.8598661626226551</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24">
+      <c r="A24" s="2">
         <f>0.025/12</f>
         <v>2.0833333333333333E-3</v>
       </c>
@@ -1300,7 +1311,7 @@
       <c r="C24">
         <v>1200</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <f t="shared" si="0"/>
         <v>87.605476419371399</v>
       </c>

</xml_diff>